<commit_message>
HW7 american option errors rerun
</commit_message>
<xml_diff>
--- a/final_preparation/FiniteDifference_ForwardEuler_HW7/HW7_Group5_graded.xlsx
+++ b/final_preparation/FiniteDifference_ForwardEuler_HW7/HW7_Group5_graded.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ericzeng/Documents/numerical-method-for-finance/MTH9821-numerical-method-for-financial-engineering/final_preparation/FiniteDifference_ForwardEuler_HW7/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F7DDF5D-2DAB-414D-AF07-AEBC90373C40}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03B3EEAF-EA14-CC4F-A6DE-47594846BF5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="4980" yWindow="5780" windowWidth="25400" windowHeight="20400" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -903,7 +903,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK1048576"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView topLeftCell="O1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
       <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
@@ -1993,7 +1993,7 @@
   <dimension ref="A1:Q46"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M45" sqref="M45"/>
+      <selection activeCell="E36" sqref="E36:K41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>

</xml_diff>